<commit_message>
Archivo de selección subido
</commit_message>
<xml_diff>
--- a/Desarrollo de proyecto/Selección/Seleccion.xlsx
+++ b/Desarrollo de proyecto/Selección/Seleccion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuel\Documents\Manuel\Universidad\2021-2\Robótica\Proyecto\Repo\Proyecto_Robotica_G2\Desarrollo de proyecto\Selección\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59284B69-F6E8-499D-9BC3-D74B6F5ADDDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CDD4CCB-361A-4870-9BC6-2944338BA804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{C0867961-A6AC-4E31-89F1-0C40D29FEF94}"/>
   </bookViews>
@@ -84,10 +84,10 @@
     <t>Alcance</t>
   </si>
   <si>
-    <t>0.58 m</t>
-  </si>
-  <si>
     <t>La capacidad de carga de 3 kg cubre la necesidad</t>
+  </si>
+  <si>
+    <t>m</t>
   </si>
 </sst>
 </file>
@@ -529,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1EF8AB6-1347-462C-846D-5525B75915AD}">
   <dimension ref="A3:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,7 +675,7 @@
       </c>
       <c r="D21" s="3"/>
       <c r="E21" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -683,7 +683,7 @@
         <v>6</v>
       </c>
       <c r="F22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -693,8 +693,11 @@
       <c r="C23" t="s">
         <v>15</v>
       </c>
-      <c r="D23" t="s">
-        <v>16</v>
+      <c r="D23">
+        <v>0.9</v>
+      </c>
+      <c r="E23" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>